<commit_message>
updated scripts to analyse new calibration and results
</commit_message>
<xml_diff>
--- a/code/COSA_Analysis/results_table.xlsx
+++ b/code/COSA_Analysis/results_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10070"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10065"/>
   </bookViews>
   <sheets>
     <sheet name="results_table" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>2050_False_100000</t>
   </si>
   <si>
-    <t>2019_False_100000</t>
-  </si>
-  <si>
-    <t>2019_True_100000</t>
-  </si>
-  <si>
-    <t>2019_True_1</t>
-  </si>
-  <si>
     <t>inst_cum_com_median</t>
   </si>
   <si>
@@ -111,18 +102,43 @@
     <t>Community adopters [-]</t>
   </si>
   <si>
-    <t>Community PV subsidies policy cost [m EUR]</t>
-  </si>
-  <si>
-    <t>Individual PV subsidies policy cost [m EUR]</t>
+    <t>2018_False_100000</t>
+  </si>
+  <si>
+    <t>2018_True_1</t>
+  </si>
+  <si>
+    <t>2018_True_100000</t>
+  </si>
+  <si>
+    <t>Total PV adoption [MWp]</t>
+  </si>
+  <si>
+    <t>Total PV subsidies policy cost [m CHF]</t>
+  </si>
+  <si>
+    <t>Community PV subsidies policy cost [m CHF]</t>
+  </si>
+  <si>
+    <t>Individual PV subsidies policy cost [m CHF]</t>
+  </si>
+  <si>
+    <t>Total adopters [-]</t>
+  </si>
+  <si>
+    <t>Policy efficiency [Wp/CHF]</t>
+  </si>
+  <si>
+    <t>Outcome\Scenario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -441,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -556,6 +572,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -601,7 +635,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,6 +650,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -661,7 +710,41 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -672,6 +755,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G1:K19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="G1:K19"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Outcome\Scenario"/>
+    <tableColumn id="2" name="IND" dataDxfId="5"/>
+    <tableColumn id="3" name="COM" dataDxfId="4"/>
+    <tableColumn id="4" name="ZEV" dataDxfId="3"/>
+    <tableColumn id="5" name="ZEV+" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,826 +1034,958 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="G1" sqref="G1:K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>3890.5</v>
-      </c>
-      <c r="D2">
-        <v>4089.5</v>
-      </c>
-      <c r="E2">
-        <v>4089.5</v>
+      <c r="B2" s="6">
+        <v>10534</v>
+      </c>
+      <c r="C2" s="6">
+        <v>6730.5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>6730.5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>6730.5</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2">
         <f>B2/1000</f>
-        <v>0</v>
+        <v>10.534000000000001</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:K2" si="0">C2/1000</f>
-        <v>3.8904999999999998</v>
+        <v>6.7305000000000001</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>4.0895000000000001</v>
+        <v>6.7305000000000001</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
-        <v>4.0895000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6.7305000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>692.5</v>
-      </c>
-      <c r="D3">
-        <v>692.5</v>
-      </c>
-      <c r="E3">
-        <v>692.5</v>
+      <c r="B3" s="6">
+        <v>7120.95</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3975.15</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4049.85</v>
+      </c>
+      <c r="E3" s="6">
+        <v>3978.3</v>
       </c>
       <c r="H3" s="1" t="str">
         <f>CONCATENATE("(",ROUND(B3/1000,1),"; ",ROUND(B4/1000,1),")")</f>
-        <v>(0; 0)</v>
+        <v>(7.1; 13.5)</v>
       </c>
       <c r="I3" s="1" t="str">
         <f t="shared" ref="I3:K3" si="1">CONCATENATE("(",ROUND(C3/1000,1),"; ",ROUND(C4/1000,1),")")</f>
-        <v>(0.7; 11.4)</v>
+        <v>(4; 9.3)</v>
       </c>
       <c r="J3" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(0.7; 12.7)</v>
+        <v>(4; 9.1)</v>
       </c>
       <c r="K3" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(0.7; 13)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>(4; 9.1)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>11397.3999999999</v>
-      </c>
-      <c r="D4">
-        <v>12731.6499999999</v>
-      </c>
-      <c r="E4">
-        <v>13018.799999999899</v>
+      <c r="B4" s="6">
+        <v>13486.75</v>
+      </c>
+      <c r="C4" s="6">
+        <v>9323.0499999999993</v>
+      </c>
+      <c r="D4" s="6">
+        <v>9084.25</v>
+      </c>
+      <c r="E4" s="6">
+        <v>9084.25</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2">
         <f>B5/1000</f>
-        <v>10.263</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ref="I4:K4" si="2">C5/1000</f>
-        <v>7.33</v>
+        <v>3.8555000000000001</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="2"/>
-        <v>7.5854999999999997</v>
+        <v>3.839</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="2"/>
-        <v>7.5854999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3.9235000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>10263</v>
-      </c>
-      <c r="C5">
-        <v>7330</v>
-      </c>
-      <c r="D5">
-        <v>7585.5</v>
-      </c>
-      <c r="E5">
-        <v>7585.5</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3855.5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3839</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3923.5</v>
       </c>
       <c r="H5" s="1" t="str">
         <f>CONCATENATE("(",ROUND(B6/1000,1),"; ",ROUND(B7/1000,1),")")</f>
-        <v>(5.6; 19.6)</v>
+        <v>(0; 0)</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" ref="I5:K5" si="3">CONCATENATE("(",ROUND(C6/1000,1),"; ",ROUND(C7/1000,1),")")</f>
-        <v>(4.2; 19.1)</v>
+        <v>(1.4; 6.8)</v>
       </c>
       <c r="J5" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>(4.3; 20)</v>
+        <v>(1.1; 7.1)</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>(4.3; 19.8)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>(1.1; 7.1)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>5588.35</v>
-      </c>
-      <c r="C6">
-        <v>4236.6000000000004</v>
-      </c>
-      <c r="D6">
-        <v>4302.95</v>
-      </c>
-      <c r="E6">
-        <v>4302.95</v>
-      </c>
-      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1402.1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1148</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1148</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="12">
         <f>B21</f>
-        <v>10.263</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" ref="I6:L6" si="4">C21</f>
-        <v>11.220499999999999</v>
-      </c>
-      <c r="J6" s="3">
+        <v>10.534000000000001</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" ref="I6:K6" si="4">C21</f>
+        <v>10.586</v>
+      </c>
+      <c r="J6" s="12">
         <f t="shared" si="4"/>
-        <v>11.675000000000001</v>
-      </c>
-      <c r="K6" s="3">
+        <v>10.5695</v>
+      </c>
+      <c r="K6" s="12">
         <f t="shared" si="4"/>
-        <v>11.675000000000001</v>
+        <v>10.654</v>
       </c>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>19629.5999999999</v>
-      </c>
-      <c r="C7">
-        <v>19141.699999999899</v>
-      </c>
-      <c r="D7">
-        <v>19958.6499999999</v>
-      </c>
-      <c r="E7">
-        <v>19778.1499999999</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6796.9</v>
+      </c>
+      <c r="D7" s="6">
+        <v>7102.9</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7102.9</v>
       </c>
       <c r="H7" s="1" t="str">
         <f>CONCATENATE("(",ROUND(B22,1),"; ",ROUND(B23,1),")")</f>
-        <v>(5.6; 19.6)</v>
+        <v>(7.1; 13.5)</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" ref="I7:K7" si="5">CONCATENATE("(",ROUND(C22,1),"; ",ROUND(C23,1),")")</f>
-        <v>(4.9; 30.5)</v>
+        <v>(5.4; 16.1)</v>
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>(5; 32.7)</v>
+        <v>(5.2; 16.2)</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>(5; 32.8)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>(5.1; 16.2)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <v>52.5</v>
-      </c>
-      <c r="E8">
-        <v>54.5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="2">
-        <f>B11</f>
-        <v>97</v>
-      </c>
-      <c r="I8" s="2">
-        <f>C11</f>
-        <v>74</v>
-      </c>
-      <c r="J8" s="2">
-        <f>D11</f>
-        <v>73.5</v>
-      </c>
-      <c r="K8" s="2">
-        <f>E11</f>
-        <v>74.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="6">
+        <v>65</v>
+      </c>
+      <c r="C8" s="6">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6">
+        <v>48</v>
+      </c>
+      <c r="E8" s="6">
+        <v>48</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="9">
+        <f>B8</f>
+        <v>65</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" ref="I8:K8" si="6">C8</f>
+        <v>48</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D9">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E9">
-        <v>4.9000000000000004</v>
+      <c r="B9" s="6">
+        <v>52.45</v>
+      </c>
+      <c r="C9" s="6">
+        <v>36.450000000000003</v>
+      </c>
+      <c r="D9" s="6">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="E9" s="6">
+        <v>35.450000000000003</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(B12,1),"; ",ROUND(B13,1),")")</f>
-        <v>(53.5; 197.2)</v>
+        <f>CONCATENATE("(",ROUND(B9,1),"; ",ROUND(B10,1),")")</f>
+        <v>(52.5; 78.6)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(C12,1),"; ",ROUND(C13,1),")")</f>
-        <v>(37.9; 326.3)</v>
+        <f t="shared" ref="I9:K9" si="7">CONCATENATE("(",ROUND(C9,1),"; ",ROUND(C10,1),")")</f>
+        <v>(36.5; 58.6)</v>
       </c>
       <c r="J9" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(D12,1),"; ",ROUND(D13,1),")")</f>
-        <v>(37; 381.2)</v>
+        <f t="shared" si="7"/>
+        <v>(35.5; 59.6)</v>
       </c>
       <c r="K9" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(E12,1),"; ",ROUND(E13,1),")")</f>
-        <v>(37; 382.7)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <f t="shared" si="7"/>
+        <v>(35.5; 59.6)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
+        <v>78.55</v>
+      </c>
+      <c r="C10" s="6">
+        <v>58.55</v>
+      </c>
+      <c r="D10" s="6">
+        <v>59.55</v>
+      </c>
+      <c r="E10" s="6">
+        <v>59.55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2">
+        <f>B11</f>
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>199.99999999999901</v>
-      </c>
-      <c r="D10">
-        <v>209.64999999999901</v>
-      </c>
-      <c r="E10">
-        <v>217.94999999999899</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="2">
-        <f>B8</f>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:K10" si="8">C11</f>
+        <v>24</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="8"/>
+        <v>24.5</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="8"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6">
         <v>0</v>
       </c>
-      <c r="I10" s="2">
-        <f>C8</f>
-        <v>50</v>
-      </c>
-      <c r="J10" s="2">
-        <f>D8</f>
-        <v>52.5</v>
-      </c>
-      <c r="K10" s="2">
-        <f>E8</f>
-        <v>54.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>97</v>
-      </c>
-      <c r="C11">
-        <v>74</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="6">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6">
+        <v>24.5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>25.5</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(B12,1),"; ",ROUND(B13,1),")")</f>
+        <v>(0; 0)</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" ref="I11:K11" si="9">CONCATENATE("(",ROUND(C12,1),"; ",ROUND(C13,1),")")</f>
+        <v>(11; 40.6)</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>(9.5; 41.6)</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>(9.5; 41.6)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="12">
+        <f>B24</f>
+        <v>65</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" ref="I12:K12" si="10">C24</f>
+        <v>72</v>
+      </c>
+      <c r="J12" s="12">
+        <f t="shared" si="10"/>
+        <v>72.5</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="10"/>
         <v>73.5</v>
       </c>
-      <c r="E11">
-        <v>74.5</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(B9,1),"; ",ROUND(B10,1),")")</f>
-        <v>(0; 0)</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(C9,1),"; ",ROUND(C10,1),")")</f>
-        <v>(4.9; 200)</v>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(D9,1),"; ",ROUND(D10,1),")")</f>
-        <v>(4.9; 209.6)</v>
-      </c>
-      <c r="K11" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(E9,1),"; ",ROUND(E10,1),")")</f>
-        <v>(4.9; 217.9)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>53.45</v>
-      </c>
-      <c r="C12">
-        <v>37.9</v>
-      </c>
-      <c r="D12">
-        <v>37</v>
-      </c>
-      <c r="E12">
-        <v>37</v>
-      </c>
-      <c r="H12" s="3">
-        <f>B24</f>
-        <v>97</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" ref="I12:K12" si="6">C24</f>
-        <v>124</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="6"/>
-        <v>126</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="6"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>197.2</v>
-      </c>
-      <c r="C13">
-        <v>326.3</v>
-      </c>
-      <c r="D13">
-        <v>381.19999999999902</v>
-      </c>
-      <c r="E13">
-        <v>382.69999999999902</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>40.549999999999997</v>
+      </c>
+      <c r="D13" s="6">
+        <v>41.55</v>
+      </c>
+      <c r="E13" s="6">
+        <v>41.55</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>CONCATENATE("(",ROUND(B25,1),"; ",ROUND(B26,1),")")</f>
-        <v>(53.5; 197.2)</v>
+        <v>(52.5; 78.6)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f t="shared" ref="I13:K13" si="7">CONCATENATE("(",ROUND(C25,1),"; ",ROUND(C26,1),")")</f>
-        <v>(42.8; 526.3)</v>
+        <f t="shared" ref="I13:K13" si="11">CONCATENATE("(",ROUND(C25,1),"; ",ROUND(C26,1),")")</f>
+        <v>(47.5; 99.1)</v>
       </c>
       <c r="J13" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>(41.9; 590.8)</v>
+        <f t="shared" si="11"/>
+        <v>(44.9; 101.1)</v>
       </c>
       <c r="K13" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>(41.9; 600.6)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <f t="shared" si="11"/>
+        <v>(44.9; 101.1)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>4185210</v>
-      </c>
-      <c r="D14">
-        <v>4524650</v>
-      </c>
-      <c r="E14">
-        <v>4524650</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="3">
-        <f>B17/1000000</f>
-        <v>30.008595</v>
-      </c>
-      <c r="I14" s="3">
-        <f>C17/1000000</f>
-        <v>23.595610000000001</v>
-      </c>
-      <c r="J14" s="3">
-        <f>D17/1000000</f>
-        <v>23.217590000000001</v>
-      </c>
-      <c r="K14" s="3">
-        <f>E17/1000000</f>
-        <v>23.115349999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="6">
+        <v>30250720</v>
+      </c>
+      <c r="C14" s="6">
+        <v>21148410</v>
+      </c>
+      <c r="D14" s="6">
+        <v>20758890</v>
+      </c>
+      <c r="E14" s="6">
+        <v>20758890</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="10">
+        <f>B14/1000000</f>
+        <v>30.250720000000001</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" ref="I14:K14" si="12">C14/1000000</f>
+        <v>21.148409999999998</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="12"/>
+        <v>20.758890000000001</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="12"/>
+        <v>20.758890000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>639265</v>
-      </c>
-      <c r="D15">
-        <v>811885</v>
-      </c>
-      <c r="E15">
-        <v>811885</v>
+      <c r="B15" s="6">
+        <v>18955610</v>
+      </c>
+      <c r="C15" s="6">
+        <v>11332600</v>
+      </c>
+      <c r="D15" s="6">
+        <v>11322310</v>
+      </c>
+      <c r="E15" s="6">
+        <v>11322310</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(B18/1000000,1),"; ",ROUND(B19/1000000,1),")")</f>
-        <v>(17.4; 46.8)</v>
+        <f>CONCATENATE("(",ROUND(B15/1000000,1),"; ",ROUND(B16/1000000,1),")")</f>
+        <v>(19; 37.7)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(C18/1000000,1),"; ",ROUND(C19/1000000,1),")")</f>
-        <v>(12.8; 36.9)</v>
+        <f t="shared" ref="I15:K15" si="13">CONCATENATE("(",ROUND(C15/1000000,1),"; ",ROUND(C16/1000000,1),")")</f>
+        <v>(11.3; 30.1)</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(D18/1000000,1),"; ",ROUND(D19/1000000,1),")")</f>
-        <v>(12.8; 37.3)</v>
+        <f t="shared" si="13"/>
+        <v>(11.3; 30)</v>
       </c>
       <c r="K15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(E18/1000000,1),"; ",ROUND(E19/1000000,1),")")</f>
-        <v>(12.7; 37.2)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <f t="shared" si="13"/>
+        <v>(11.3; 30)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
+        <v>37748480</v>
+      </c>
+      <c r="C16" s="6">
+        <v>30132910</v>
+      </c>
+      <c r="D16" s="6">
+        <v>30028100</v>
+      </c>
+      <c r="E16" s="6">
+        <v>30028100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="3">
+        <f>B17/1000000</f>
         <v>0</v>
       </c>
-      <c r="C16">
-        <v>11528799.999999899</v>
-      </c>
-      <c r="D16">
-        <v>12434961.999999899</v>
-      </c>
-      <c r="E16">
-        <v>12486584.999999899</v>
-      </c>
-      <c r="G16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="2">
-        <f>B14/1000000</f>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:K16" si="14">C17/1000000</f>
+        <v>7.784764</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="14"/>
+        <v>8.4424460000000003</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="14"/>
+        <v>8.4424460000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6">
         <v>0</v>
       </c>
-      <c r="I16" s="2">
-        <f>C14/1000000</f>
-        <v>4.1852099999999997</v>
-      </c>
-      <c r="J16" s="2">
-        <f>D14/1000000</f>
-        <v>4.5246500000000003</v>
-      </c>
-      <c r="K16" s="2">
-        <f>E14/1000000</f>
-        <v>4.5246500000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>30008595</v>
-      </c>
-      <c r="C17">
-        <v>23595610</v>
-      </c>
-      <c r="D17">
-        <v>23217590</v>
-      </c>
-      <c r="E17">
-        <v>23115350</v>
+      <c r="C17" s="6">
+        <v>7784764</v>
+      </c>
+      <c r="D17" s="6">
+        <v>8442446</v>
+      </c>
+      <c r="E17" s="6">
+        <v>8442446</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(B15/1000000,1),"; ",ROUND(B16/1000000,1),")")</f>
+        <f>CONCATENATE("(",ROUND(B18/1000000,1),"; ",ROUND(B19/1000000,1),")")</f>
         <v>(0; 0)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(C15/1000000,1),"; ",ROUND(C16/1000000,1),")")</f>
-        <v>(0.6; 11.5)</v>
+        <f t="shared" ref="I17:K17" si="15">CONCATENATE("(",ROUND(C18/1000000,1),"; ",ROUND(C19/1000000,1),")")</f>
+        <v>(2.2; 17.2)</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(D15/1000000,1),"; ",ROUND(D16/1000000,1),")")</f>
-        <v>(0.8; 12.4)</v>
+        <f t="shared" si="15"/>
+        <v>(2.4; 17.7)</v>
       </c>
       <c r="K17" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(E15/1000000,1),"; ",ROUND(E16/1000000,1),")")</f>
-        <v>(0.8; 12.5)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="15"/>
+        <v>(2.4; 17.7)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>17420328</v>
-      </c>
-      <c r="C18">
-        <v>12838452</v>
-      </c>
-      <c r="D18">
-        <v>12768573</v>
-      </c>
-      <c r="E18">
-        <v>12733149</v>
-      </c>
-      <c r="H18" s="3">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2169938</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2371824</v>
+      </c>
+      <c r="E18" s="6">
+        <v>2371824</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="12">
         <f>B27/1000000</f>
-        <v>30.008595</v>
-      </c>
-      <c r="I18" s="3">
-        <f t="shared" ref="I18:K18" si="8">C27/1000000</f>
-        <v>27.780819999999999</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="8"/>
-        <v>27.742239999999999</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="8"/>
-        <v>27.64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>30.250720000000001</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" ref="I18:K18" si="16">C27/1000000</f>
+        <v>28.933174000000001</v>
+      </c>
+      <c r="J18" s="12">
+        <f t="shared" si="16"/>
+        <v>29.201336000000001</v>
+      </c>
+      <c r="K18" s="12">
+        <f t="shared" si="16"/>
+        <v>29.201336000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>46820315</v>
-      </c>
-      <c r="C19">
-        <v>36873933.499999903</v>
-      </c>
-      <c r="D19">
-        <v>37305674.999999903</v>
-      </c>
-      <c r="E19">
-        <v>37248749.999999903</v>
+        <v>15</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>17203790</v>
+      </c>
+      <c r="D19" s="6">
+        <v>17681280</v>
+      </c>
+      <c r="E19" s="6">
+        <v>17681280</v>
       </c>
       <c r="H19" s="1" t="str">
         <f>CONCATENATE("(",ROUND(B28/1000000,1),"; ",ROUND(B29/1000000,1),")")</f>
-        <v>(17.4; 46.8)</v>
+        <v>(19; 37.7)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" ref="I19:K19" si="9">CONCATENATE("(",ROUND(C28/1000000,1),"; ",ROUND(C29/1000000,1),")")</f>
-        <v>(13.5; 48.4)</v>
+        <f t="shared" ref="I19:K19" si="17">CONCATENATE("(",ROUND(C28/1000000,1),"; ",ROUND(C29/1000000,1),")")</f>
+        <v>(13.5; 47.3)</v>
       </c>
       <c r="J19" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>(13.6; 49.7)</v>
+        <f t="shared" si="17"/>
+        <v>(13.7; 47.7)</v>
       </c>
       <c r="K19" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>(13.5; 49.7)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="17"/>
+        <v>(13.7; 47.7)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="7">
+        <f>H6/H18</f>
+        <v>0.34822311667292549</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" ref="I20:K20" si="18">I6/I18</f>
+        <v>0.36587759089272404</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="18"/>
+        <v>0.36195261751037688</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="18"/>
+        <v>0.36484632072998302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <f>(B2+B5)/1000</f>
-        <v>10.263</v>
+        <v>10.534000000000001</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" ref="C21:E21" si="10">(C2+C5)/1000</f>
-        <v>11.220499999999999</v>
+        <f t="shared" ref="C21:E21" si="19">(C2+C5)/1000</f>
+        <v>10.586</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="10"/>
-        <v>11.675000000000001</v>
+        <f t="shared" si="19"/>
+        <v>10.5695</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="10"/>
-        <v>11.675000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="19"/>
+        <v>10.654</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <f t="shared" ref="B22:E23" si="11">(B3+B6)/1000</f>
-        <v>5.5883500000000002</v>
+        <f t="shared" ref="B22:E23" si="20">(B3+B6)/1000</f>
+        <v>7.1209499999999997</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="11"/>
-        <v>4.9291</v>
+        <f t="shared" si="20"/>
+        <v>5.3772500000000001</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="11"/>
-        <v>4.9954499999999999</v>
+        <f t="shared" si="20"/>
+        <v>5.1978500000000007</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="11"/>
-        <v>4.9954499999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="20"/>
+        <v>5.1263000000000005</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
-        <f t="shared" si="11"/>
-        <v>19.6295999999999</v>
+        <f t="shared" si="20"/>
+        <v>13.486750000000001</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="11"/>
-        <v>30.539099999999799</v>
+        <f t="shared" si="20"/>
+        <v>16.119949999999999</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="11"/>
-        <v>32.690299999999802</v>
+        <f t="shared" si="20"/>
+        <v>16.187149999999999</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="11"/>
-        <v>32.796949999999804</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="20"/>
+        <v>16.187149999999999</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
         <f>(B11+B8)</f>
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" ref="C24:E24" si="12">(C11+C8)</f>
-        <v>124</v>
+        <f t="shared" ref="C24:E24" si="21">(C11+C8)</f>
+        <v>72</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="12"/>
-        <v>126</v>
+        <f t="shared" si="21"/>
+        <v>72.5</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="12"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="21"/>
+        <v>73.5</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <f t="shared" ref="B25:E25" si="13">(B12+B9)</f>
-        <v>53.45</v>
+        <f t="shared" ref="B25:E25" si="22">(B12+B9)</f>
+        <v>52.45</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="13"/>
-        <v>42.8</v>
+        <f t="shared" si="22"/>
+        <v>47.45</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="13"/>
-        <v>41.9</v>
+        <f t="shared" si="22"/>
+        <v>44.900000000000006</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="13"/>
-        <v>41.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="22"/>
+        <v>44.900000000000006</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
-        <f t="shared" ref="B26:E26" si="14">(B13+B10)</f>
-        <v>197.2</v>
+        <f t="shared" ref="B26:E26" si="23">(B13+B10)</f>
+        <v>78.55</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="14"/>
-        <v>526.29999999999905</v>
+        <f t="shared" si="23"/>
+        <v>99.1</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="14"/>
-        <v>590.84999999999809</v>
+        <f t="shared" si="23"/>
+        <v>101.1</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="14"/>
-        <v>600.64999999999804</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="23"/>
+        <v>101.1</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <f>(B14+B17)</f>
-        <v>30008595</v>
+        <v>30250720</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" ref="C27:E27" si="15">(C14+C17)</f>
-        <v>27780820</v>
+        <f t="shared" ref="C27:E27" si="24">(C14+C17)</f>
+        <v>28933174</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="15"/>
-        <v>27742240</v>
+        <f t="shared" si="24"/>
+        <v>29201336</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="15"/>
-        <v>27640000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="24"/>
+        <v>29201336</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
-        <f t="shared" ref="B28:E29" si="16">(B15+B18)</f>
-        <v>17420328</v>
+        <f t="shared" ref="B28:E29" si="25">(B15+B18)</f>
+        <v>18955610</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="16"/>
-        <v>13477717</v>
+        <f t="shared" si="25"/>
+        <v>13502538</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="16"/>
-        <v>13580458</v>
+        <f t="shared" si="25"/>
+        <v>13694134</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="16"/>
-        <v>13545034</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="25"/>
+        <v>13694134</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
-        <f t="shared" si="16"/>
-        <v>46820315</v>
+        <f t="shared" si="25"/>
+        <v>37748480</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="16"/>
-        <v>48402733.499999806</v>
+        <f t="shared" si="25"/>
+        <v>47336700</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="16"/>
-        <v>49740636.999999806</v>
+        <f t="shared" si="25"/>
+        <v>47709380</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="16"/>
-        <v>49735334.999999806</v>
-      </c>
+        <f t="shared" si="25"/>
+        <v>47709380</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H20:K20">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>